<commit_message>
updats on last commit
</commit_message>
<xml_diff>
--- a/data/uploads/sea.xlsx
+++ b/data/uploads/sea.xlsx
@@ -2594,11 +2594,11 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>LDJD035</t>
+          <t>LDJD0333</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>600</v>
+        <v>333</v>
       </c>
       <c r="C83" t="n">
         <v>642.9059999999999</v>

</xml_diff>